<commit_message>
lots of data cleaning
</commit_message>
<xml_diff>
--- a/Masculinity_Data_Dictionary.xlsx
+++ b/Masculinity_Data_Dictionary.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie\GA Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie\GA Final Project\Masculinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0EFF103-8574-46AC-A114-2E6F4A6654C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C824C465-1475-46B2-9A8A-9AFB834940B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8745" xr2:uid="{17B072F3-1DFB-4E60-B900-748577D567B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cleaning needed" sheetId="2" r:id="rId1"/>
+    <sheet name="Dictionary" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cleaning needed'!$A$1:$F$98</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="163">
   <si>
     <t>StartDate</t>
   </si>
@@ -321,38 +325,6 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>In general, how masculine or "manly" do you feel?
-Very masculine, Somewhat masculine, Not very masculine, Not at all masculine, No answer</t>
-  </si>
-  <si>
-    <t>How important is it to you that others see you as masculine?
-Very important, Somewhat important, Not too important, Not at all important, No answer</t>
-  </si>
-  <si>
-    <t>Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
-Response = Father or father figure(s)</t>
-  </si>
-  <si>
-    <t>Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
-Response = Mother or mother figure(s)</t>
-  </si>
-  <si>
-    <t>Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
-Response = Friends</t>
-  </si>
-  <si>
-    <t>Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
-Response = Other family members</t>
-  </si>
-  <si>
-    <t>Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
-Response = Pop culture</t>
-  </si>
-  <si>
-    <t>Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
-Response = Other</t>
-  </si>
-  <si>
     <t>Do you think that society puts pressure on men in a way that is unhealthy or bad for them?</t>
   </si>
   <si>
@@ -360,13 +332,202 @@
   </si>
   <si>
     <t>How often do you ask a friend for personal advice?</t>
+  </si>
+  <si>
+    <t>How often do you express physical affection to male friends, like hugging, rubbing shoulders?</t>
+  </si>
+  <si>
+    <t>How often do you cry?</t>
+  </si>
+  <si>
+    <t>How often do you get in a physical fight with another person?</t>
+  </si>
+  <si>
+    <t>How often do you have sexual relations with women, including anything from kissing to sex?</t>
+  </si>
+  <si>
+    <t>How often do you have sexual relations with men, including anything from kissing to sex?</t>
+  </si>
+  <si>
+    <t>How often do you watch sports of any kind?</t>
+  </si>
+  <si>
+    <t>How often do you work out?</t>
+  </si>
+  <si>
+    <t>How often do you see a therapist?</t>
+  </si>
+  <si>
+    <t>How often do you feel lonely or isolated</t>
+  </si>
+  <si>
+    <t>Response options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In general, how masculine or "manly" do you feel?
+</t>
+  </si>
+  <si>
+    <t>Very masculine, Somewhat masculine, Not very masculine, Not at all masculine, No answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How important is it to you that others see you as masculine?
+</t>
+  </si>
+  <si>
+    <t>Very important, Somewhat important, Not too important, Not at all important, No answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where have you gotten your ideas about what it means to be a good man? (Select all that apply.) 
+</t>
+  </si>
+  <si>
+    <t>Response = Father or father figure(s)</t>
+  </si>
+  <si>
+    <t>Response = Mother or mother figure(s)</t>
+  </si>
+  <si>
+    <t>Response = Friends</t>
+  </si>
+  <si>
+    <t>Response = Other family members</t>
+  </si>
+  <si>
+    <t>Response = Pop culture</t>
+  </si>
+  <si>
+    <t>Response = Other</t>
+  </si>
+  <si>
+    <t>Yes, No, No answer</t>
+  </si>
+  <si>
+    <t>Often, Sometimes, Rarely, Never but open to it, Never and not open to it</t>
+  </si>
+  <si>
+    <t>Which of the following do you worry about on a daily or near daily basis? (Select all that apply)</t>
+  </si>
+  <si>
+    <t>Your height</t>
+  </si>
+  <si>
+    <t>Your weight</t>
+  </si>
+  <si>
+    <t>Your physique</t>
+  </si>
+  <si>
+    <t>Your hair or hairline</t>
+  </si>
+  <si>
+    <t>Appearance of your genitalia</t>
+  </si>
+  <si>
+    <t>Your clothing or style</t>
+  </si>
+  <si>
+    <t>Sexual performance or amount of sex</t>
+  </si>
+  <si>
+    <t>Your mental health</t>
+  </si>
+  <si>
+    <t>Your physical health</t>
+  </si>
+  <si>
+    <t>Your finances, including your current or future assets or debt</t>
+  </si>
+  <si>
+    <t>Your ability to provide for your family, current or anticipated</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Which of the following categories best describes your employment status?</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employed working full time, Employed working part time, Not employed-student, Not employed-retired, Not employed- looking for work, Not employed NOT looking for work </t>
+  </si>
+  <si>
+    <t>Cleaning needed</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Need to fill 2 null vals</t>
+  </si>
+  <si>
+    <t>Need to fill 20 null vals</t>
+  </si>
+  <si>
+    <t>Not interesting/ relevant</t>
+  </si>
+  <si>
+    <t>Weird dummy-like columns, not relevant</t>
+  </si>
+  <si>
+    <t>Unsure</t>
+  </si>
+  <si>
+    <t>me_too_romantic_behavior</t>
+  </si>
+  <si>
+    <t>Need to filter on respondents who answered this question to make predictions on it (742)</t>
+  </si>
+  <si>
+    <t>Use (Y/N?)</t>
+  </si>
+  <si>
+    <t>Num N/A</t>
+  </si>
+  <si>
+    <t>Drop NA</t>
+  </si>
+  <si>
+    <t>If no answer for all, then drop line?</t>
+  </si>
+  <si>
+    <t>In which of the following ways would you say it's an advantage to be a man at work right now?</t>
+  </si>
+  <si>
+    <t>In which of the following ways would you say it's a disadvantage to be a man at work right now?</t>
+  </si>
+  <si>
+    <t>Have you seen or heard of a secual harassment incident at your work? If so, how did you respond?</t>
+  </si>
+  <si>
+    <t>How much have you heard about the #MeToo movement?</t>
+  </si>
+  <si>
+    <t>Do you typically feel as though you're expected to make the first move in romantic relationships?</t>
+  </si>
+  <si>
+    <t>How often do you try to be the one who pays when on a date?</t>
+  </si>
+  <si>
+    <t>If using, would need to filter on always or often above</t>
+  </si>
+  <si>
+    <t>When you want to be physically intimate with someone how do you gauge their interest?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,13 +543,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -403,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -413,6 +596,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -728,521 +920,1895 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B39A8F8-4641-4AC1-BC63-6701DACE289A}">
+  <dimension ref="A1:F98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="2">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F98" xr:uid="{6DBECCEF-8E6B-4EFC-A4DA-D927E8C08114}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA34643-17AE-476D-9DDF-572304A537E4}">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="135.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="38" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
drop NA vals, wrote more explanation markdown
</commit_message>
<xml_diff>
--- a/Masculinity_Data_Dictionary.xlsx
+++ b/Masculinity_Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie\GA Final Project\Masculinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C824C465-1475-46B2-9A8A-9AFB834940B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD13AF84-465C-4D5C-964A-B69791B516C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8745" xr2:uid="{17B072F3-1DFB-4E60-B900-748577D567B2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="170">
   <si>
     <t>StartDate</t>
   </si>
@@ -496,18 +496,12 @@
     <t>Drop NA</t>
   </si>
   <si>
-    <t>If no answer for all, then drop line?</t>
-  </si>
-  <si>
     <t>In which of the following ways would you say it's an advantage to be a man at work right now?</t>
   </si>
   <si>
     <t>In which of the following ways would you say it's a disadvantage to be a man at work right now?</t>
   </si>
   <si>
-    <t>Have you seen or heard of a secual harassment incident at your work? If so, how did you respond?</t>
-  </si>
-  <si>
     <t>How much have you heard about the #MeToo movement?</t>
   </si>
   <si>
@@ -521,6 +515,33 @@
   </si>
   <si>
     <t>When you want to be physically intimate with someone how do you gauge their interest?</t>
+  </si>
+  <si>
+    <t>1- Create new col to flag no answer for any col</t>
+  </si>
+  <si>
+    <t>2-Create new col to flag no answer for any col</t>
+  </si>
+  <si>
+    <t>3- Create new col to flag no answer for any col</t>
+  </si>
+  <si>
+    <t>4- Create new col to flag no answer for any col</t>
+  </si>
+  <si>
+    <t>Have you seen or heard of a sexual harassment incident at your work? If so, how did you respond?</t>
+  </si>
+  <si>
+    <t>Only answered by a small subset of respondents</t>
+  </si>
+  <si>
+    <t>5- Create new col to flag no answer for any col</t>
+  </si>
+  <si>
+    <t>6- Create new col to flag no answer for any col</t>
+  </si>
+  <si>
+    <t>7- Create new col to flag no answer for any col</t>
   </si>
 </sst>
 </file>
@@ -923,13 +944,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B39A8F8-4641-4AC1-BC63-6701DACE289A}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="3" width="4.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.140625" style="2" customWidth="1"/>
@@ -1010,7 +1031,7 @@
         <v>140</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>115</v>
@@ -1027,7 +1048,7 @@
         <v>140</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>115</v>
@@ -1044,7 +1065,7 @@
         <v>140</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>115</v>
@@ -1061,7 +1082,7 @@
         <v>140</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>115</v>
@@ -1078,7 +1099,7 @@
         <v>140</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>115</v>
@@ -1095,7 +1116,7 @@
         <v>140</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>115</v>
@@ -1316,7 +1337,7 @@
         <v>140</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>124</v>
@@ -1333,7 +1354,7 @@
         <v>140</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>126</v>
@@ -1347,7 +1368,7 @@
         <v>140</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>128</v>
@@ -1361,7 +1382,7 @@
         <v>140</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>127</v>
@@ -1375,7 +1396,7 @@
         <v>140</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>129</v>
@@ -1389,7 +1410,7 @@
         <v>140</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>130</v>
@@ -1403,7 +1424,7 @@
         <v>140</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>131</v>
@@ -1417,7 +1438,7 @@
         <v>140</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>132</v>
@@ -1431,7 +1452,7 @@
         <v>140</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>133</v>
@@ -1445,7 +1466,7 @@
         <v>140</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>134</v>
@@ -1459,7 +1480,7 @@
         <v>140</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>135</v>
@@ -1473,7 +1494,7 @@
         <v>140</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>136</v>
@@ -1498,10 +1519,10 @@
         <v>35</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1509,7 +1530,7 @@
         <v>36</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1517,7 +1538,7 @@
         <v>37</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1525,7 +1546,7 @@
         <v>38</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1533,7 +1554,7 @@
         <v>39</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,7 +1562,7 @@
         <v>40</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1549,7 +1570,7 @@
         <v>41</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1557,7 +1578,7 @@
         <v>42</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,10 +1586,10 @@
         <v>43</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1576,7 +1597,7 @@
         <v>44</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1584,7 +1605,7 @@
         <v>45</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1592,7 +1613,7 @@
         <v>46</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1600,46 +1621,67 @@
         <v>47</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="D50" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="E50" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="D51" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="52" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="D52" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="53" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="D53" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="54" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D54" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="56" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="D56" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="57" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
@@ -1648,13 +1690,16 @@
       <c r="B57" s="7" t="s">
         <v>139</v>
       </c>
+      <c r="E57" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="58" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1673,7 +1718,7 @@
         <v>58</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,7 +1730,7 @@
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1697,7 +1742,7 @@
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1754,7 @@
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1721,7 +1766,7 @@
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,7 +1778,7 @@
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1745,7 +1790,7 @@
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1757,7 +1802,7 @@
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1769,7 +1814,7 @@
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1779,8 +1824,11 @@
       <c r="B69" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D69" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="E69" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1790,6 +1838,9 @@
       <c r="B70" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D70" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="71" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
@@ -1798,6 +1849,9 @@
       <c r="B71" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D71" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="72" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
@@ -1806,6 +1860,9 @@
       <c r="B72" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D72" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="73" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -1814,6 +1871,9 @@
       <c r="B73" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D73" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="74" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
@@ -1822,6 +1882,9 @@
       <c r="B74" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D74" s="2" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="75" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
@@ -1830,6 +1893,9 @@
       <c r="B75" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D75" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="76" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
@@ -1838,6 +1904,9 @@
       <c r="B76" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D76" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="77" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
@@ -1846,6 +1915,9 @@
       <c r="B77" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D77" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="78" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
@@ -1854,6 +1926,9 @@
       <c r="B78" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="D78" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="79" spans="1:5" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
@@ -1950,101 +2025,110 @@
       </c>
     </row>
     <row r="90" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="C90" s="7"/>
+      <c r="D90" s="7" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="C91" s="7"/>
+      <c r="D91" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="C92" s="7"/>
+      <c r="D92" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="C93" s="7"/>
+      <c r="D93" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="C94" s="7"/>
+      <c r="D94" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="C95" s="7"/>
+      <c r="D95" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="C96" s="7"/>
+      <c r="D96" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="C97" s="7"/>
+      <c r="D97" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="C98" s="7"/>
+      <c r="D98" s="7" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
attempted to map values and test for skips
</commit_message>
<xml_diff>
--- a/Masculinity_Data_Dictionary.xlsx
+++ b/Masculinity_Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie\GA Final Project\Masculinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{67ED6E1C-17B5-4ED4-AEDE-A907640EC8F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8561A27A-0274-41F0-99E7-0E603329D558}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8745" xr2:uid="{17B072F3-1DFB-4E60-B900-748577D567B2}"/>
   </bookViews>
@@ -1001,18 +1001,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B39A8F8-4641-4AC1-BC63-6701DACE289A}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="3" width="3.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="6" width="4.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="68.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
loop to map multi-response questions to 1s and 0s, create T/F columns to flag lines that did skipped the questions
</commit_message>
<xml_diff>
--- a/Masculinity_Data_Dictionary.xlsx
+++ b/Masculinity_Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie\GA Final Project\Masculinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8561A27A-0274-41F0-99E7-0E603329D558}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6C18E545-01AD-4405-9A10-178F2B1F980C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8745" xr2:uid="{17B072F3-1DFB-4E60-B900-748577D567B2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="183">
   <si>
     <t>StartDate</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>Drop column completely</t>
+  </si>
+  <si>
+    <t>men_more_praise</t>
   </si>
 </sst>
 </file>
@@ -643,7 +646,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -651,11 +654,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -683,6 +704,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -999,11 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B39A8F8-4641-4AC1-BC63-6701DACE289A}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1039,7 @@
     <col min="2" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="6" width="4.140625" customWidth="1"/>
-    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="7" max="7" width="65.5703125" customWidth="1"/>
     <col min="8" max="8" width="68.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2007,7 +2034,7 @@
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>39</v>
+        <v>182</v>
       </c>
       <c r="B41" s="2">
         <v>40</v>
@@ -2066,22 +2093,24 @@
       </c>
     </row>
     <row r="44" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="11">
         <v>43</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="11">
         <v>10</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="11" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2165,7 +2194,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -2185,27 +2214,31 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="50" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="12">
         <v>49</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="12">
         <v>12</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="12" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -2225,7 +2258,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
@@ -2245,7 +2278,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -2265,7 +2298,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -2285,7 +2318,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2305,7 +2338,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -2325,7 +2358,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>55</v>
       </c>
@@ -2348,7 +2381,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
@@ -2365,7 +2398,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>77</v>
       </c>
@@ -2385,7 +2418,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -2399,7 +2432,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
@@ -2417,7 +2450,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>60</v>
       </c>
@@ -2436,7 +2469,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>61</v>
       </c>
@@ -2455,7 +2488,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
tested self-manly and others-manly
</commit_message>
<xml_diff>
--- a/Masculinity_Data_Dictionary.xlsx
+++ b/Masculinity_Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephanie\GA Final Project\Masculinity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{057D045B-7A4A-4F5A-B987-A8E0ADD3E32C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5732E15-5B2D-4C0F-B448-73BBD8E44819}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8745" xr2:uid="{17B072F3-1DFB-4E60-B900-748577D567B2}"/>
   </bookViews>
@@ -1036,8 +1036,8 @@
   <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G86" sqref="G86"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>